<commit_message>
memperbaiki export import manage name
</commit_message>
<xml_diff>
--- a/management_name_list.xlsx
+++ b/management_name_list.xlsx
@@ -491,22 +491,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>coba</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>test@gmail.com</t>
+          <t>cb@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Perempuan</t>
+          <t>Laki-laki</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>testt</t>
+          <t>pertanian</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -514,12 +514,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>f5fbc6fe84c365315f491d4275c2f2e5d3c60f25684e1d62e7e9fe63abf8d0d8</t>
+          <t>12345678</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>f5fbc6fe84c365315f491d4275c2f2e5d3c60f25684e1d62e7e9fe63abf8d0d8</t>
+          <t>12345678</t>
         </is>
       </c>
     </row>
@@ -534,22 +534,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>jjl</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>jajal@gmail.com</t>
+          <t>test@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Laki-laki</t>
+          <t>Perempuan</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>dkv</t>
+          <t>testt</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -557,12 +557,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>jajal1234</t>
+          <t>f5fbc6fe84c365315f491d4275c2f2e5d3c60f25684e1d62e7e9fe63abf8d0d8</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>jajal1234</t>
+          <t>f5fbc6fe84c365315f491d4275c2f2e5d3c60f25684e1d62e7e9fe63abf8d0d8</t>
         </is>
       </c>
     </row>
@@ -663,22 +663,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>erfer</t>
+          <t>jjl</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>tes@gmail.com</t>
+          <t>jajal@gmail.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>laki</t>
+          <t>Laki-laki</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>tbsm</t>
+          <t>dkv</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -686,12 +686,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>aveceenaintifadhafirdausming</t>
+          <t>jajal1234</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>aveceenaintifadhafirdausming</t>
+          <t>jajal1234</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>hihi</t>
+          <t>erfer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>hi@gmail.com</t>
+          <t>tes@gmail.com</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>tkj</t>
+          <t>tbsm</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -729,12 +729,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>aveceena123</t>
+          <t>aveceenaintifadhafirdausming</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>aveceena123</t>
+          <t>aveceenaintifadhafirdausming</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>hihi</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>p@gmail.com</t>
+          <t>hi@gmail.com</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Laki</t>
+          <t>laki</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -772,12 +772,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>39cc70ddc804005a99b5c9be676f9b550cb3482c57467b05dc88d48857dd7aa3</t>
+          <t>aveceena123</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>39cc70ddc804005a99b5c9be676f9b550cb3482c57467b05dc88d48857dd7aa3</t>
+          <t>aveceena123</t>
         </is>
       </c>
     </row>
@@ -792,17 +792,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>testing</t>
+          <t>p</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>test@gmail.com</t>
+          <t>p@gmail.com</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>perempuan</t>
+          <t>Laki</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>8bb0cf6eb9b17d0f7d22b456f121257dc1254e1f01665370476383ea776df414</t>
+          <t>39cc70ddc804005a99b5c9be676f9b550cb3482c57467b05dc88d48857dd7aa3</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>8bb0cf6eb9b17d0f7d22b456f121257dc1254e1f01665370476383ea776df414</t>
+          <t>39cc70ddc804005a99b5c9be676f9b550cb3482c57467b05dc88d48857dd7aa3</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>080835910</t>
+          <t>080835901</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -871,26 +871,42 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>080835910</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>v</t>
+          <t>testing</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>v@gmail.com</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>perempuan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>tkj</t>
+        </is>
+      </c>
       <c r="G11" t="n">
         <v>5</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>8bb0cf6eb9b17d0f7d22b456f121257dc1254e1f01665370476383ea776df414</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>39cc70ddc804005a99b5c9be676f9b550cb3482c57467b05dc88d48857dd7aa3</t>
+          <t>8bb0cf6eb9b17d0f7d22b456f121257dc1254e1f01665370476383ea776df414</t>
         </is>
       </c>
     </row>

</xml_diff>